<commit_message>
GET TESTS -Share test
</commit_message>
<xml_diff>
--- a/checklist.xlsx
+++ b/checklist.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Sofia/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Sofia/Documents/desktop-testverktyg/verktyg-server/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t xml:space="preserve">Som lärare vill jag kunna ställa olika typer av frågor i testverktyget (ex. flervalsfrågor, alternativfrågor, öppna frågor, rangordningsfrågor) </t>
   </si>
@@ -68,22 +68,40 @@
     <t xml:space="preserve">Som administratör/lärare/utbildningsledare vill jag kunna få statistik över testresultatet (antal godkända, medelvärde, hur lång tid testet tog etc.) för samtliga testgrupper </t>
   </si>
   <si>
+    <t>Matilda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Användarhistorier </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ansvarig </t>
+  </si>
+  <si>
+    <t>Kommentar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slutdatum </t>
+  </si>
+  <si>
+    <t>Ändra alla knappar, labels,textfield. De ska skapas av klassen CreateNodes</t>
+  </si>
+  <si>
     <t>Sofia</t>
   </si>
   <si>
-    <t>Matilda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Användarhistorier </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ansvarig </t>
-  </si>
-  <si>
-    <t>Kommentar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slutdatum </t>
+    <t>Markus</t>
+  </si>
+  <si>
+    <t>Shuffla svarsalternativ när användaren skriver ett prov</t>
+  </si>
+  <si>
+    <t>Philip</t>
+  </si>
+  <si>
+    <t>Ta bort navbar vid utloggning</t>
+  </si>
+  <si>
+    <t>kommentera kod</t>
   </si>
 </sst>
 </file>
@@ -104,7 +122,7 @@
       <name val="Times New Roman"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -132,6 +150,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -148,12 +178,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -164,6 +193,17 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -454,16 +494,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
         <v>16</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -477,11 +517,11 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -490,62 +530,91 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="7" t="s">
         <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="6" t="s">
         <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="9"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GET Students -Share test
</commit_message>
<xml_diff>
--- a/checklist.xlsx
+++ b/checklist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t xml:space="preserve">Som lärare vill jag kunna ställa olika typer av frågor i testverktyget (ex. flervalsfrågor, alternativfrågor, öppna frågor, rangordningsfrågor) </t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>kommentera kod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ny sida när testet är skapat/alternativt meddelande </t>
   </si>
 </sst>
 </file>
@@ -481,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -617,6 +620,11 @@
         <v>24</v>
       </c>
     </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
GET Students -Share test -UPDATE
</commit_message>
<xml_diff>
--- a/checklist.xlsx
+++ b/checklist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t xml:space="preserve">Som lärare vill jag kunna ställa olika typer av frågor i testverktyget (ex. flervalsfrågor, alternativfrågor, öppna frågor, rangordningsfrågor) </t>
   </si>
@@ -105,6 +105,12 @@
   </si>
   <si>
     <t xml:space="preserve">Ny sida när testet är skapat/alternativt meddelande </t>
+  </si>
+  <si>
+    <t>Skapa ny användare - lägg till mejl</t>
+  </si>
+  <si>
+    <t>När man skiftar mellan sidor sparas datan (fråga Sofia)</t>
   </si>
 </sst>
 </file>
@@ -484,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -625,6 +631,16 @@
         <v>25</v>
       </c>
     </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
query - UTest update
</commit_message>
<xml_diff>
--- a/checklist.xlsx
+++ b/checklist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t xml:space="preserve">Som lärare vill jag kunna ställa olika typer av frågor i testverktyget (ex. flervalsfrågor, alternativfrågor, öppna frågor, rangordningsfrågor) </t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>När man skiftar mellan sidor sparas datan (fråga Sofia)</t>
+  </si>
+  <si>
+    <t>fel medd när man försöker reg  användare 2 ggr</t>
   </si>
 </sst>
 </file>
@@ -490,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -638,6 +641,11 @@
         <v>27</v>
       </c>
     </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
query - PDF update
</commit_message>
<xml_diff>
--- a/checklist.xlsx
+++ b/checklist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t xml:space="preserve">Som lärare vill jag kunna ställa olika typer av frågor i testverktyget (ex. flervalsfrågor, alternativfrågor, öppna frågor, rangordningsfrågor) </t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>fel medd när man försöker reg  användare 2 ggr</t>
+  </si>
+  <si>
+    <t>Dela till gruppen</t>
   </si>
 </sst>
 </file>
@@ -134,7 +137,7 @@
       <name val="Times New Roman"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -156,12 +159,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -190,12 +187,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -205,15 +201,12 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
@@ -496,7 +489,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="A27" sqref="A26:A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -529,12 +522,12 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B5" t="s">
@@ -547,7 +540,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -557,7 +550,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -567,20 +560,23 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>20</v>
       </c>
+      <c r="D12" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B13" t="s">
@@ -588,28 +584,28 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="9"/>
+    <row r="16" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="7"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="10" t="s">
         <v>21</v>
       </c>
       <c r="B18" t="s">
@@ -617,32 +613,32 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="9" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="10" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="10" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="9" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="9" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>